<commit_message>
updating xpath of selling price in view details and ErrorScreenshot position
</commit_message>
<xml_diff>
--- a/provide/Output/OutputDataProvide.xlsx
+++ b/provide/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -225,12 +225,22 @@
   </si>
   <si>
     <t>99</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,12 +289,32 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -315,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -332,6 +362,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -613,40 +645,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AG1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" customWidth="1"/>
-    <col min="18" max="18" width="26" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
-    <col min="22" max="23" width="15.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="19.7109375" customWidth="1"/>
-    <col min="29" max="29" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" width="17.140625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="22" max="23" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="26" max="28" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -743,6 +775,9 @@
       <c r="AE1" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -838,6 +873,9 @@
       <c r="AE2" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="AG2" t="s" s="12">
+        <v>58</v>
+      </c>
     </row>
     <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -932,6 +970,9 @@
       </c>
       <c r="AE3" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="AG3" t="s" s="13">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>